<commit_message>
Also import klass teachers when importing students
</commit_message>
<xml_diff>
--- a/stages/test_files/CLOEE2_Export_FE_2018.xlsx
+++ b/stages/test_files/CLOEE2_Export_FE_2018.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="133">
   <si>
     <t xml:space="preserve">ELE_NUMERO</t>
   </si>
@@ -121,6 +121,9 @@
     <t xml:space="preserve">CTRT_CODE_CANTON</t>
   </si>
   <si>
+    <t xml:space="preserve">INS_MC</t>
+  </si>
+  <si>
     <t xml:space="preserve">ENT_NUMERO</t>
   </si>
   <si>
@@ -289,6 +292,9 @@
     <t xml:space="preserve">2ASSCFEa</t>
   </si>
   <si>
+    <t xml:space="preserve">Dupond Jeanne</t>
+  </si>
+  <si>
     <t xml:space="preserve">Centre Cantonal de peinture</t>
   </si>
   <si>
@@ -359,6 +365,9 @@
   </si>
   <si>
     <t xml:space="preserve">2EDEpe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dupond Jeanne, Secrétariat EPC Secrétariat EPC</t>
   </si>
   <si>
     <t xml:space="preserve">101</t>
@@ -420,7 +429,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -453,6 +462,12 @@
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -498,7 +513,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -516,6 +531,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -538,11 +557,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="false" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="U1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AE5" activeCellId="0" sqref="AE5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Z1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AH4" activeCellId="0" sqref="AH4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.39"/>
@@ -559,17 +578,19 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="22.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="20.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="31.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="19" style="0" width="8.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="40.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="37" style="0" width="8.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="38.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="40" style="0" width="8.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="0" width="16.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="44" style="0" width="8.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="0" width="16.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="49" style="0" width="8.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="0" width="23.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="52" style="0" width="8.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="19" style="0" width="8.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="32.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="35" style="0" width="8.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="40.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="38" style="0" width="8.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="38.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="41" style="0" width="8.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="0" width="16.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="45" style="0" width="8.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="0" width="16.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="50" style="0" width="8.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="52" style="0" width="23.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="53" style="0" width="8.52"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -777,8 +798,10 @@
       <c r="BP1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="BR1" s="2"/>
-      <c r="BT1" s="2"/>
+      <c r="BQ1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="BS1" s="2"/>
       <c r="BU1" s="2"/>
       <c r="BV1" s="2"/>
       <c r="BW1" s="2"/>
@@ -790,8 +813,8 @@
       <c r="CC1" s="2"/>
       <c r="CD1" s="2"/>
       <c r="CE1" s="2"/>
-      <c r="AHZ1" s="2"/>
-      <c r="AIA1" s="0"/>
+      <c r="CF1" s="2"/>
+      <c r="AIA1" s="2"/>
       <c r="AIB1" s="0"/>
       <c r="AIC1" s="0"/>
       <c r="AID1" s="0"/>
@@ -911,143 +934,145 @@
         <v>11111</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="J2" s="3"/>
       <c r="K2" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L2" s="3"/>
       <c r="M2" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="P2" s="3"/>
       <c r="Q2" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="U2" s="3"/>
       <c r="V2" s="3"/>
       <c r="W2" s="3"/>
       <c r="X2" s="3"/>
       <c r="Y2" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AC2" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD2" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="AD2" s="3" t="s">
-        <v>86</v>
-      </c>
       <c r="AE2" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AF2" s="3"/>
       <c r="AG2" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="AH2" s="2" t="n">
+        <v>78</v>
+      </c>
+      <c r="AH2" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="AI2" s="2" t="n">
         <v>100</v>
       </c>
-      <c r="AI2" s="3"/>
-      <c r="AJ2" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="AK2" s="3"/>
-      <c r="AL2" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="AM2" s="4" t="s">
+      <c r="AJ2" s="3"/>
+      <c r="AK2" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="AN2" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="AO2" s="3"/>
-      <c r="AP2" s="3" t="s">
+      <c r="AL2" s="3"/>
+      <c r="AM2" s="3" t="s">
         <v>92</v>
       </c>
+      <c r="AN2" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="AO2" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="AP2" s="3"/>
       <c r="AQ2" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AR2" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="AS2" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AT2" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AU2" s="3" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="AV2" s="3" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="AW2" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="AX2" s="2" t="n">
+        <v>99</v>
+      </c>
+      <c r="AX2" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="AY2" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="AY2" s="3"/>
       <c r="AZ2" s="3"/>
-      <c r="BB2" s="3"/>
-      <c r="BC2" s="3" t="s">
-        <v>77</v>
-      </c>
+      <c r="BA2" s="3"/>
+      <c r="BC2" s="3"/>
       <c r="BD2" s="3" t="s">
-        <v>99</v>
+        <v>78</v>
       </c>
       <c r="BE2" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="BF2" s="3"/>
+        <v>101</v>
+      </c>
+      <c r="BF2" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="BG2" s="3"/>
       <c r="BH2" s="3"/>
       <c r="BI2" s="3"/>
@@ -1058,7 +1083,7 @@
       <c r="BN2" s="3"/>
       <c r="BO2" s="3"/>
       <c r="BP2" s="3"/>
-      <c r="AIA2" s="0"/>
+      <c r="BQ2" s="3"/>
       <c r="AIB2" s="0"/>
       <c r="AIC2" s="0"/>
       <c r="AID2" s="0"/>
@@ -1178,93 +1203,95 @@
         <v>22222</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="L3" s="3"/>
       <c r="M3" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="P3" s="3"/>
       <c r="Q3" s="3" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="T3" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="U3" s="3"/>
       <c r="V3" s="3"/>
       <c r="W3" s="3"/>
       <c r="X3" s="3"/>
       <c r="Y3" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="Z3" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="AA3" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="AB3" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AC3" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD3" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="AD3" s="3" t="s">
-        <v>86</v>
-      </c>
       <c r="AE3" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="AF3" s="3"/>
       <c r="AG3" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="AH3" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="AI3" s="3"/>
-      <c r="AJ3" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="AK3" s="3"/>
+        <v>78</v>
+      </c>
+      <c r="AH3" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="AI3" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="AJ3" s="3"/>
+      <c r="AK3" s="3" t="s">
+        <v>117</v>
+      </c>
       <c r="AL3" s="3"/>
       <c r="AM3" s="3"/>
       <c r="AN3" s="3"/>
@@ -1275,10 +1302,10 @@
       <c r="AS3" s="3"/>
       <c r="AT3" s="3"/>
       <c r="AU3" s="3"/>
-      <c r="AV3" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="AW3" s="3"/>
+      <c r="AV3" s="3"/>
+      <c r="AW3" s="3" t="s">
+        <v>118</v>
+      </c>
       <c r="AX3" s="3"/>
       <c r="AY3" s="3"/>
       <c r="AZ3" s="3"/>
@@ -1298,97 +1325,98 @@
       <c r="BN3" s="3"/>
       <c r="BO3" s="3"/>
       <c r="BP3" s="3"/>
+      <c r="BQ3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
         <v>33333</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="L4" s="3"/>
       <c r="M4" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="P4" s="3"/>
       <c r="Q4" s="3" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="R4" s="3"/>
       <c r="S4" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="U4" s="3"/>
       <c r="V4" s="3"/>
       <c r="W4" s="3"/>
       <c r="X4" s="3"/>
       <c r="Y4" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="AB4" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AC4" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD4" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="AD4" s="3" t="s">
-        <v>86</v>
-      </c>
       <c r="AE4" s="3" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="AF4" s="3"/>
       <c r="AG4" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="AH4" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="AI4" s="3"/>
-      <c r="AJ4" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="AK4" s="3"/>
+        <v>78</v>
+      </c>
+      <c r="AH4" s="3"/>
+      <c r="AI4" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="AJ4" s="3"/>
+      <c r="AK4" s="3" t="s">
+        <v>131</v>
+      </c>
       <c r="AL4" s="3"/>
       <c r="AM4" s="3"/>
       <c r="AN4" s="3"/>
@@ -1399,10 +1427,10 @@
       <c r="AS4" s="3"/>
       <c r="AT4" s="3"/>
       <c r="AU4" s="3"/>
-      <c r="AV4" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="AW4" s="3"/>
+      <c r="AV4" s="3"/>
+      <c r="AW4" s="3" t="s">
+        <v>132</v>
+      </c>
       <c r="AX4" s="3"/>
       <c r="AY4" s="3"/>
       <c r="AZ4" s="3"/>
@@ -1422,10 +1450,11 @@
       <c r="BN4" s="3"/>
       <c r="BO4" s="3"/>
       <c r="BP4" s="3"/>
+      <c r="BQ4" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="AM2" r:id="rId1" display="info.cnp@ne.ch"/>
+    <hyperlink ref="AN2" r:id="rId1" display="info.cnp@ne.ch"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Updated FE Export test file
</commit_message>
<xml_diff>
--- a/stages/test_files/CLOEE2_Export_FE_2018.xlsx
+++ b/stages/test_files/CLOEE2_Export_FE_2018.xlsx
@@ -394,7 +394,7 @@
     <t xml:space="preserve">Rue de la Chaume</t>
   </si>
   <si>
-    <t xml:space="preserve">2300 Genève</t>
+    <t xml:space="preserve">FR-25140 Charquemont</t>
   </si>
   <si>
     <t xml:space="preserve">CLOEE</t>
@@ -540,12 +540,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -557,11 +557,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Z1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AH4" activeCellId="0" sqref="AH4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.39"/>

</xml_diff>